<commit_message>
se refactorizo la seleccion de los legajos desde la BD. Se agrega el casteo para los operarios normales tambien. Se agrega el color verde para los registros casteados.
</commit_message>
<xml_diff>
--- a/Archivos de trabajo/A completar/Rechazados/Rechazados 2020-10-01 al 2020-10-15.xlsx
+++ b/Archivos de trabajo/A completar/Rechazados/Rechazados 2020-10-01 al 2020-10-15.xlsx
@@ -16,7 +16,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -56,11 +61,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -426,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,6 +513,206 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>703</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JAIME EMANUEL ES </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Viernes</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>44120</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>44120.38958333333</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>44120.66736111111</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>44120</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>44120</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <v>44120</v>
+      </c>
+      <c r="J2" s="3" t="n">
+        <v>44120</v>
+      </c>
+      <c r="K2" s="3" t="n">
+        <v>44120</v>
+      </c>
+      <c r="L2" s="3" t="n">
+        <v>44120</v>
+      </c>
+      <c r="M2" s="3" t="n">
+        <v>44120</v>
+      </c>
+      <c r="N2" s="3" t="n">
+        <v>44120</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>703</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JAIME EMANUEL ES </t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Sábado</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>44121</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>44121.32430555556</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>44121.66736111111</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>44121</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>44121</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>44121</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>44121</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>44121</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>44121</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>44121</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <v>44121</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>705</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BALMACEDA FRANCO NICOLAS DR </t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Viernes</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>44120</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>44120.38541666666</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>44120.54166666666</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>44120.56180555555</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>44120.7</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>44120</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>44120</v>
+      </c>
+      <c r="K4" s="3" t="n">
+        <v>44120</v>
+      </c>
+      <c r="L4" s="3" t="n">
+        <v>44120</v>
+      </c>
+      <c r="M4" s="3" t="n">
+        <v>44120</v>
+      </c>
+      <c r="N4" s="3" t="n">
+        <v>44120</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>706</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PERALTA MARIO ALBERTO RE </t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Viernes</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>44120</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>44120.39166666667</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>44120.52291666667</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>44120.54027777778</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>44120.70208333333</v>
+      </c>
+      <c r="I5" s="3" t="n">
+        <v>44120</v>
+      </c>
+      <c r="J5" s="3" t="n">
+        <v>44120</v>
+      </c>
+      <c r="K5" s="3" t="n">
+        <v>44120</v>
+      </c>
+      <c r="L5" s="3" t="n">
+        <v>44120</v>
+      </c>
+      <c r="M5" s="3" t="n">
+        <v>44120</v>
+      </c>
+      <c r="N5" s="3" t="n">
+        <v>44120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agregaron 2 columnas a las tablas, se agregan los dias que no hay registros como 00, solo se sube a la BD si no hay registros en rojo
</commit_message>
<xml_diff>
--- a/Archivos de trabajo/A completar/Rechazados/Rechazados 2020-10-01 al 2020-10-15.xlsx
+++ b/Archivos de trabajo/A completar/Rechazados/Rechazados 2020-10-01 al 2020-10-15.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,7 +444,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Empleado</t>
+          <t>Legajo</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -510,6 +510,16 @@
       <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Egreso_4</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Motivo</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Observación</t>
         </is>
       </c>
     </row>
@@ -562,6 +572,8 @@
       <c r="N2" s="3" t="n">
         <v>44120</v>
       </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -612,6 +624,8 @@
       <c r="N3" s="3" t="n">
         <v>44121</v>
       </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -662,6 +676,8 @@
       <c r="N4" s="3" t="n">
         <v>44120</v>
       </c>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -712,6 +728,8 @@
       <c r="N5" s="3" t="n">
         <v>44120</v>
       </c>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Cambios a 8,8 horas. Nuevas columnas de retraso y tardanza, nuevas opciones para eleccion de falta. Cambio previo a hacer la seleccion del motivo y hacer el cambio en la hoja
</commit_message>
<xml_diff>
--- a/Archivos de trabajo/A completar/Rechazados/Rechazados 2020-10-01 al 2020-10-15.xlsx
+++ b/Archivos de trabajo/A completar/Rechazados/Rechazados 2020-10-01 al 2020-10-15.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,12 +526,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>703</t>
+          <t>705</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">JAIME EMANUEL ES </t>
+          <t xml:space="preserve">BALMACEDA FRANCO NICOLAS DR </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -543,16 +543,16 @@
         <v>44120</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>44120.38958333333</v>
+        <v>44120.38541666666</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>44120.66736111111</v>
+        <v>44120.54166666666</v>
       </c>
       <c r="G2" s="3" t="n">
-        <v>44120</v>
+        <v>44120.56180555555</v>
       </c>
       <c r="H2" s="3" t="n">
-        <v>44120</v>
+        <v>44120.7</v>
       </c>
       <c r="I2" s="3" t="n">
         <v>44120</v>
@@ -578,158 +578,54 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>703</t>
+          <t>706</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">JAIME EMANUEL ES </t>
+          <t xml:space="preserve">PERALTA MARIO ALBERTO RE </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Sábado</t>
+          <t>Viernes</t>
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>44121</v>
+        <v>44120</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>44121.32430555556</v>
+        <v>44120.39166666667</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>44121.66736111111</v>
+        <v>44120.52291666667</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>44121</v>
+        <v>44120.54027777778</v>
       </c>
       <c r="H3" s="3" t="n">
-        <v>44121</v>
+        <v>44120.70208333333</v>
       </c>
       <c r="I3" s="3" t="n">
-        <v>44121</v>
+        <v>44120</v>
       </c>
       <c r="J3" s="3" t="n">
-        <v>44121</v>
+        <v>44120</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>44121</v>
+        <v>44120</v>
       </c>
       <c r="L3" s="3" t="n">
-        <v>44121</v>
+        <v>44120</v>
       </c>
       <c r="M3" s="3" t="n">
-        <v>44121</v>
+        <v>44120</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>44121</v>
+        <v>44120</v>
       </c>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>705</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">BALMACEDA FRANCO NICOLAS DR </t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Viernes</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>44120</v>
-      </c>
-      <c r="E4" s="3" t="n">
-        <v>44120.38541666666</v>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>44120.54166666666</v>
-      </c>
-      <c r="G4" s="3" t="n">
-        <v>44120.56180555555</v>
-      </c>
-      <c r="H4" s="3" t="n">
-        <v>44120.7</v>
-      </c>
-      <c r="I4" s="3" t="n">
-        <v>44120</v>
-      </c>
-      <c r="J4" s="3" t="n">
-        <v>44120</v>
-      </c>
-      <c r="K4" s="3" t="n">
-        <v>44120</v>
-      </c>
-      <c r="L4" s="3" t="n">
-        <v>44120</v>
-      </c>
-      <c r="M4" s="3" t="n">
-        <v>44120</v>
-      </c>
-      <c r="N4" s="3" t="n">
-        <v>44120</v>
-      </c>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>706</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PERALTA MARIO ALBERTO RE </t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Viernes</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>44120</v>
-      </c>
-      <c r="E5" s="3" t="n">
-        <v>44120.39166666667</v>
-      </c>
-      <c r="F5" s="3" t="n">
-        <v>44120.52291666667</v>
-      </c>
-      <c r="G5" s="3" t="n">
-        <v>44120.54027777778</v>
-      </c>
-      <c r="H5" s="3" t="n">
-        <v>44120.70208333333</v>
-      </c>
-      <c r="I5" s="3" t="n">
-        <v>44120</v>
-      </c>
-      <c r="J5" s="3" t="n">
-        <v>44120</v>
-      </c>
-      <c r="K5" s="3" t="n">
-        <v>44120</v>
-      </c>
-      <c r="L5" s="3" t="n">
-        <v>44120</v>
-      </c>
-      <c r="M5" s="3" t="n">
-        <v>44120</v>
-      </c>
-      <c r="N5" s="3" t="n">
-        <v>44120</v>
-      </c>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>